<commit_message>
Lab 5 Dice Game finished ,code left bugs...Unable to overcome the problems in transfromming SM graph to SM statements
</commit_message>
<xml_diff>
--- a/OtherFiles/DE2_70_pin_assignments.xlsx
+++ b/OtherFiles/DE2_70_pin_assignments.xlsx
@@ -4226,12 +4226,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E552"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" topLeftCell="A309" workbookViewId="0">
+      <selection activeCell="D320" sqref="D320"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="17.625" customWidth="1"/>
     <col min="2" max="2" width="15.875" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>